<commit_message>
HP updated week 1 material
</commit_message>
<xml_diff>
--- a/CourseStructrure_AY2024-25.xlsx
+++ b/CourseStructrure_AY2024-25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/mg13730_bristol_ac_uk/Documents/Teaching/2024/FCP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/hp12384_bristol_ac_uk/Documents/Teaching/UoB/EMAT10007_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4BDC61E-409A-46B4-AC70-9F201600FD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{E4BDC61E-409A-46B4-AC70-9F201600FD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91C1A48F-4EEE-3349-B04A-310163C66C61}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB69D0A4-597B-4DBB-A11D-3E8D6AA8DFB6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{EB69D0A4-597B-4DBB-A11D-3E8D6AA8DFB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>Summative coursework due</t>
-  </si>
-  <si>
-    <t>Vivas?</t>
   </si>
   <si>
     <t>Summative coursework released</t>
@@ -343,31 +340,49 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -684,405 +699,401 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9138578E-7460-4A95-82D6-FE3AF5733998}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="105.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5" style="14" customWidth="1"/>
+    <col min="6" max="6" width="37.1640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="3" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>6</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="16" t="s">
         <v>43</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>8</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>9</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="3" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="16" t="s">
         <v>44</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>11</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="3" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="16" t="s">
         <v>38</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="4">
         <v>12</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="4"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="18"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>13</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="16" t="s">
         <v>39</v>
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>15</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="3" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>16</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="3" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>17</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="3" t="s">
+      <c r="C19" s="12"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="16" t="s">
         <v>35</v>
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>18</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>19</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="16" t="s">
         <v>40</v>
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>20</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="3" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="16"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <v>21</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="3" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="16" t="s">
         <v>42</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <v>22</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="3">
         <v>23</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
+      <c r="D25" s="10"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16" t="s">
         <v>41</v>
       </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
         <v>24</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
       <c r="G26" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G27" t="s">
-        <v>54</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="D24:D26"/>
     <mergeCell ref="D3:D7"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HP updated week 2
</commit_message>
<xml_diff>
--- a/CourseStructrure_AY2024-25.xlsx
+++ b/CourseStructrure_AY2024-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/hp12384_bristol_ac_uk/Documents/Teaching/UoB/EMAT10007_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{E4BDC61E-409A-46B4-AC70-9F201600FD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91C1A48F-4EEE-3349-B04A-310163C66C61}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{E4BDC61E-409A-46B4-AC70-9F201600FD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F261AB5-87DA-AE41-8088-72893E1E648C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{EB69D0A4-597B-4DBB-A11D-3E8D6AA8DFB6}"/>
   </bookViews>
@@ -62,18 +62,9 @@
     <t>Programming Fundamentals</t>
   </si>
   <si>
-    <t xml:space="preserve">Intro </t>
-  </si>
-  <si>
-    <t>Variables &amp; Operators</t>
-  </si>
-  <si>
     <t>Seminar 1 - algorithms</t>
   </si>
   <si>
-    <t>Control flow</t>
-  </si>
-  <si>
     <t>Loops</t>
   </si>
   <si>
@@ -207,6 +198,15 @@
   </si>
   <si>
     <t>Consolidation 1 - Turtlesim? Text-based adventure game?</t>
+  </si>
+  <si>
+    <t>Intro, variables and arithmetic and assignment operators</t>
+  </si>
+  <si>
+    <t>Comparison, identity and logical Operators</t>
+  </si>
+  <si>
+    <t>Control flow (if, elif, else)</t>
   </si>
 </sst>
 </file>
@@ -350,21 +350,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -383,6 +368,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -400,6 +400,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -702,15 +706,15 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5" style="14" customWidth="1"/>
-    <col min="6" max="6" width="37.1640625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="36.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="37.1640625" style="9" customWidth="1"/>
     <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -728,31 +732,31 @@
       <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>10</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -760,27 +764,27 @@
       <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="16"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="11"/>
       <c r="G4" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>13</v>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -788,27 +792,27 @@
       <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="16"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="11"/>
       <c r="G6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>14</v>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -820,27 +824,27 @@
         <v>6</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>43</v>
+      <c r="C9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -848,27 +852,27 @@
       <c r="B10" s="3">
         <v>8</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="11"/>
       <c r="G10" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>9</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>44</v>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -876,46 +880,46 @@
       <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="16"/>
+      <c r="C12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="11"/>
       <c r="G12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>11</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>38</v>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="4">
         <v>12</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="18"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="13"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -924,11 +928,11 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -936,29 +940,29 @@
       <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="D16" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="11"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>15</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>34</v>
+      <c r="C17" s="15"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -966,27 +970,27 @@
       <c r="B18" s="3">
         <v>16</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="16"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="11"/>
       <c r="G18" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>17</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>35</v>
+      <c r="C19" s="15"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -998,8 +1002,8 @@
         <v>6</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="2:7" ht="16" x14ac:dyDescent="0.2">
@@ -1007,14 +1011,14 @@
         <v>19</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>40</v>
+      <c r="D21" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1023,11 +1027,11 @@
         <v>20</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="16"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="11"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="2:7" ht="32" x14ac:dyDescent="0.2">
@@ -1035,15 +1039,15 @@
         <v>21</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>42</v>
+      <c r="D23" s="18"/>
+      <c r="E23" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -1051,9 +1055,9 @@
         <v>22</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="2:7" ht="16" x14ac:dyDescent="0.2">
@@ -1061,10 +1065,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16" t="s">
-        <v>41</v>
+      <c r="D25" s="16"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1073,25 +1077,25 @@
         <v>24</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
       <c r="G26" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D14"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C16:C19"/>
     <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
HP added wk 12 material@
</commit_message>
<xml_diff>
--- a/CourseStructrure_AY2024-25.xlsx
+++ b/CourseStructrure_AY2024-25.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/hp12384_bristol_ac_uk/Documents/Teaching/UoB/EMAT10007_2023_/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/hp12384_bristol_ac_uk/Documents/Teaching/UoB/EMAT10007_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{E4BDC61E-409A-46B4-AC70-9F201600FD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F261AB5-87DA-AE41-8088-72893E1E648C}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="8_{E4BDC61E-409A-46B4-AC70-9F201600FD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9108BFEC-E512-40EB-9EC8-2B3E41401300}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{EB69D0A4-597B-4DBB-A11D-3E8D6AA8DFB6}"/>
+    <workbookView xWindow="37620" yWindow="-3020" windowWidth="28800" windowHeight="18780" firstSheet="1" activeTab="1" xr2:uid="{EB69D0A4-597B-4DBB-A11D-3E8D6AA8DFB6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v1" sheetId="1" r:id="rId1"/>
+    <sheet name="v2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="87">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -44,6 +45,9 @@
     <t>Week 1</t>
   </si>
   <si>
+    <t>Concept</t>
+  </si>
+  <si>
     <t>Theme</t>
   </si>
   <si>
@@ -53,52 +57,130 @@
     <t>Seminar</t>
   </si>
   <si>
-    <t>Concept</t>
+    <t>Assessments</t>
+  </si>
+  <si>
+    <t>Algorithms and the notional machine</t>
+  </si>
+  <si>
+    <t>Programming Fundamentals</t>
+  </si>
+  <si>
+    <t>Intro, variables and arithmetic and assignment operators</t>
+  </si>
+  <si>
+    <t>Seminar 1 - algorithms</t>
+  </si>
+  <si>
+    <t>Comparison, identity and logical Operators</t>
+  </si>
+  <si>
+    <t>CA1</t>
+  </si>
+  <si>
+    <t>Control flow (if, elif, else)</t>
+  </si>
+  <si>
+    <t>Seminar 2 - notional machine</t>
+  </si>
+  <si>
+    <t>Loops</t>
+  </si>
+  <si>
+    <t>CA2</t>
+  </si>
+  <si>
+    <t>Consolidation 1 - Turtlesim? Text-based adventure game?</t>
+  </si>
+  <si>
+    <t>Seminar 3 - debugging</t>
   </si>
   <si>
     <t>Reading week</t>
   </si>
   <si>
-    <t>Programming Fundamentals</t>
-  </si>
-  <si>
-    <t>Seminar 1 - algorithms</t>
-  </si>
-  <si>
-    <t>Loops</t>
-  </si>
-  <si>
-    <t>Seminar 2 - notional machine</t>
-  </si>
-  <si>
-    <t>Seminar 3 - debugging</t>
+    <t>CA3</t>
+  </si>
+  <si>
+    <t>Teach yourself</t>
+  </si>
+  <si>
+    <t>Working with data</t>
   </si>
   <si>
     <t>Data Structures (Lists)</t>
   </si>
   <si>
-    <t>Working with data</t>
+    <t>Seminar 4 - Terminals, notebooks, IDEs</t>
   </si>
   <si>
     <t>Reading data, Matplotlib</t>
   </si>
   <si>
+    <t>CA4</t>
+  </si>
+  <si>
+    <t>Consolidation 2 - descriptive statistics of a data set (w/ independent use of a python module for statistical analysis)</t>
+  </si>
+  <si>
+    <t>Seminar 5 - Writing readable code</t>
+  </si>
+  <si>
+    <t>Decomposition</t>
+  </si>
+  <si>
     <t>Writing code that works</t>
   </si>
   <si>
+    <t>Functions 1 (define, returning)</t>
+  </si>
+  <si>
+    <t>CA5</t>
+  </si>
+  <si>
     <t>Functions 2 (scope)</t>
   </si>
   <si>
-    <t>Functions 1 (define, returning)</t>
-  </si>
-  <si>
-    <t>Algorithms and the notional machine</t>
-  </si>
-  <si>
-    <t>Teach yourself</t>
-  </si>
-  <si>
-    <t>Consolidation 2 - descriptive statistics of a data set (w/ independent use of a python module for statistical analysis)</t>
+    <t>Seminar 6 - Testing and ChatGPT</t>
+  </si>
+  <si>
+    <t>Final submission for CA</t>
+  </si>
+  <si>
+    <t>Consolidation 3 - Refactoring and extending code</t>
+  </si>
+  <si>
+    <t>Post-Christmas Refresher (&amp; Dicts?)</t>
+  </si>
+  <si>
+    <t>Seminar 7 - Organising code with functions</t>
+  </si>
+  <si>
+    <t>Abstraction</t>
+  </si>
+  <si>
+    <t>Understanding and implementing algorithms</t>
+  </si>
+  <si>
+    <t>Trees , graphs and networks</t>
+  </si>
+  <si>
+    <t>Searching and sorting?</t>
+  </si>
+  <si>
+    <t>Seminar 8 - Algorithmic complexity</t>
+  </si>
+  <si>
+    <t>OOP</t>
+  </si>
+  <si>
+    <t>Formative coursework</t>
+  </si>
+  <si>
+    <t>Consolidation 4 - Game of life? Solve a maze?</t>
+  </si>
+  <si>
+    <t>Seminar 9 - Lists vs Dicts vs Arrays</t>
   </si>
   <si>
     <t>Writing code for modelling</t>
@@ -107,113 +189,177 @@
     <t>Numpy</t>
   </si>
   <si>
+    <t>Seminar 10 - Debugging 3</t>
+  </si>
+  <si>
     <t>Numpy 2</t>
   </si>
   <si>
-    <t>Understanding and implementing algorithms</t>
-  </si>
-  <si>
-    <t>OOP</t>
-  </si>
-  <si>
-    <t>Trees , graphs and networks</t>
-  </si>
-  <si>
-    <t>Searching and sorting?</t>
-  </si>
-  <si>
-    <t>Consolidation 4 - Game of life? Solve a maze?</t>
-  </si>
-  <si>
-    <t>Abstraction</t>
-  </si>
-  <si>
-    <t>Decomposition</t>
-  </si>
-  <si>
-    <t>Seminar 8 - Algorithmic complexity</t>
-  </si>
-  <si>
-    <t>Seminar 9 - Lists vs Dicts vs Arrays</t>
-  </si>
-  <si>
-    <t>Post-Christmas Refresher (&amp; Dicts?)</t>
-  </si>
-  <si>
     <t>Consolidation 5: ODE model</t>
   </si>
   <si>
-    <t>Seminar 6 - Testing and ChatGPT</t>
-  </si>
-  <si>
-    <t>Seminar 7 - Organising code with functions</t>
-  </si>
-  <si>
-    <t>Seminar 10 - Debugging 3</t>
+    <t>Seminar 11 - Libraries you should know about (SciPy, Pandas, SKLearn, etc)</t>
+  </si>
+  <si>
+    <t>Summative coursework released</t>
   </si>
   <si>
     <t>Seminar 12</t>
   </si>
   <si>
-    <t>Seminar 11 - Libraries you should know about (SciPy, Pandas, SKLearn, etc)</t>
-  </si>
-  <si>
-    <t>Seminar 4 - Terminals, notebooks, IDEs</t>
-  </si>
-  <si>
-    <t>Seminar 5 - Writing readable code</t>
-  </si>
-  <si>
-    <t>Assessments</t>
-  </si>
-  <si>
-    <t>CA1</t>
-  </si>
-  <si>
-    <t>CA2</t>
-  </si>
-  <si>
-    <t>CA3</t>
-  </si>
-  <si>
-    <t>CA4</t>
-  </si>
-  <si>
-    <t>CA5</t>
-  </si>
-  <si>
-    <t>Final submission for CA</t>
-  </si>
-  <si>
-    <t>Formative coursework</t>
-  </si>
-  <si>
     <t>Summative coursework due</t>
   </si>
   <si>
-    <t>Summative coursework released</t>
-  </si>
-  <si>
-    <t>Consolidation 3 - Refactoring and extending code</t>
-  </si>
-  <si>
-    <t>Consolidation 1 - Turtlesim? Text-based adventure game?</t>
-  </si>
-  <si>
-    <t>Intro, variables and arithmetic and assignment operators</t>
-  </si>
-  <si>
-    <t>Comparison, identity and logical Operators</t>
-  </si>
-  <si>
-    <t>Control flow (if, elif, else)</t>
+    <t>Seminar 1 - Algorithms</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Seminar 2 - Notional machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Consolidation 1 - Text-based adventure game</t>
+  </si>
+  <si>
+    <t>Seminar 3 - Debugging 1</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Seminar 4 - Different environments: Terminals, notebooks, IDEs</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Consolidation 2 - descriptive statistics of a data set (w/ independent use of a python module for statistical analysis) + feedback Consolidation 1</t>
+  </si>
+  <si>
+    <t>Seminar 5 - Style and structure: Writing readable code</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>Consolidation 3 - Refactoring and extending code (ODE model? SIR?) + feedback Consolidation 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post-Christmas Refresher 
+Intro to algorithms + Numpy </t>
+  </si>
+  <si>
+    <t>Seminar 11 - Libraries you should know about (Numpy SciPy, Pandas, SKLearn, etc)</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>Searching and sorting</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>Consolidation 4 - Game of life? Solve a maze? + feedback Consolidation 3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Summative code portfolio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> submission (P1-6)</t>
+    </r>
+  </si>
+  <si>
+    <t>CW support</t>
+  </si>
+  <si>
+    <t>Seminar 10 - Debugging 2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Summative coursework </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">released
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Seminar 7 - Version control?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Summative coursework</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> submission</t>
+    </r>
+  </si>
+  <si>
+    <t>Enrichment session: Modelling, ODE?</t>
+  </si>
+  <si>
+    <t>Viva</t>
+  </si>
+  <si>
+    <t>Enrichment session: Modellng - Discrete?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrichment session: Modelling, Agent based - Turtlesim? </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,8 +381,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,8 +419,14 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -334,13 +506,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -362,26 +560,95 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -400,10 +667,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -705,21 +968,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9138578E-7460-4A95-82D6-FE3AF5733998}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5" style="9" customWidth="1"/>
-    <col min="6" max="6" width="37.1640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.95" thickBot="1"/>
+    <row r="2" spans="1:7" ht="17.100000000000001" thickBot="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -727,377 +990,799 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>4</v>
-      </c>
       <c r="G2" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="32.1">
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="37" t="s">
         <v>7</v>
       </c>
+      <c r="D3" s="37" t="s">
+        <v>8</v>
+      </c>
       <c r="E3" s="11" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.95">
       <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="11" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.95">
       <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="11" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.95">
       <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="32.1">
       <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="11" t="s">
-        <v>53</v>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="B8" s="3">
         <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.95">
       <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>13</v>
+      <c r="C9" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>22</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.95">
       <c r="B10" s="3">
         <v>8</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="11" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="48">
       <c r="B11" s="3">
         <v>9</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="11" t="s">
-        <v>20</v>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15.95">
       <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>15</v>
-      </c>
       <c r="E12" s="11" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.95">
       <c r="B13" s="3">
         <v>11</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="11" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" ht="32.1">
       <c r="B14" s="4">
         <v>12</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="13"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="22"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.95">
       <c r="B15" s="3">
         <v>13</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15.95">
       <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>24</v>
+      <c r="C16" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>40</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="15.95">
       <c r="B17" s="3">
         <v>15</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="17"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="11" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="15.95">
       <c r="B18" s="3">
         <v>16</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="11" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="15.95">
       <c r="B19" s="3">
         <v>17</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="11" t="s">
-        <v>28</v>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7">
       <c r="B20" s="3">
         <v>18</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="15.95">
       <c r="B21" s="3">
         <v>19</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="18" t="s">
-        <v>21</v>
+      <c r="D21" s="34" t="s">
+        <v>48</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="15.95">
       <c r="B22" s="3">
         <v>20</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="18"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="11" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="32.1">
       <c r="B23" s="3">
         <v>21</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="18"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="11" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
       <c r="B24" s="3">
         <v>22</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="16"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="15.95">
       <c r="B25" s="3">
         <v>23</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="16"/>
+      <c r="D25" s="35"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="15.95" thickBot="1">
       <c r="B26" s="5">
         <v>24</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="D24:D26"/>
     <mergeCell ref="D3:D7"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0470AA-90DD-BA45-ACA6-FD07B49C07BC}">
+  <dimension ref="B1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" customWidth="1"/>
+    <col min="5" max="5" width="42" customWidth="1"/>
+    <col min="6" max="6" width="37.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.95" thickBot="1"/>
+    <row r="2" spans="2:7" ht="17.100000000000001" thickBot="1">
+      <c r="B2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="32.1">
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="2:7" ht="15.95">
+      <c r="B4" s="16">
+        <v>2</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="26"/>
+      <c r="G4" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.95">
+      <c r="B5" s="16">
+        <v>3</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.95">
+      <c r="B6" s="16">
+        <v>4</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.95">
+      <c r="B7" s="16">
+        <v>5</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="16">
+        <v>6</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="32.1">
+      <c r="B9" s="16">
+        <v>7</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.95">
+      <c r="B10" s="16">
+        <v>8</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="48">
+      <c r="B11" s="16">
+        <v>9</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.95">
+      <c r="B12" s="16">
+        <v>10</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="2:7" ht="15.95">
+      <c r="B13" s="16">
+        <v>11</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="32.1">
+      <c r="B14" s="20">
+        <v>12</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="32.1">
+      <c r="B15" s="16">
+        <v>13</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.95">
+      <c r="B16" s="16">
+        <v>14</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="26"/>
+      <c r="G16" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15.95">
+      <c r="B17" s="16">
+        <v>15</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="15.95">
+      <c r="B18" s="16">
+        <v>16</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="26"/>
+      <c r="G18" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30.75">
+      <c r="B19" s="16">
+        <v>17</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="16">
+        <v>18</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="2:7" ht="75.95" customHeight="1">
+      <c r="B21" s="16">
+        <v>19</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15.95">
+      <c r="B22" s="16">
+        <v>20</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="2:7" ht="32.1">
+      <c r="B23" s="16">
+        <v>21</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="15.95">
+      <c r="B24" s="16">
+        <v>22</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="15.95">
+      <c r="B25" s="16">
+        <v>23</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="33" thickBot="1">
+      <c r="B26" s="21">
+        <v>24</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="29"/>
+      <c r="G26" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>